<commit_message>
se corren las primeras pruebas de MATLAB-ARDUINO
</commit_message>
<xml_diff>
--- a/robotica-fija/serial_settings.xlsx
+++ b/robotica-fija/serial_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ing-Electronica-ITCG\ing-electronica-itcg\robotica-fija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6618A8EC-2231-4688-AD96-D50108329086}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2CBEE6-47AD-40E9-8B79-F9167AC0359C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages Arduino - MatLab" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>Error code</t>
   </si>
@@ -175,15 +175,9 @@
     <t>d</t>
   </si>
   <si>
-    <t>Attach or Detecha an specific servo</t>
-  </si>
-  <si>
     <t>d3,0</t>
   </si>
   <si>
-    <t>Detach ELBOW servo (1 attach and put HOME_DEGREE)</t>
-  </si>
-  <si>
     <t>No available state (only 0 or 1) (detach or attach)</t>
   </si>
   <si>
@@ -212,6 +206,15 @@
   </si>
   <si>
     <t>Test ELBOW by 10 milisecond between degree</t>
+  </si>
+  <si>
+    <t>Detach ELBOW servo (1 attach and put HOME_DEGREE, 0 dettach)</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Attach or Detech an specific servo</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -436,10 +439,16 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -448,9 +457,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,7 +484,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -808,7 +814,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,10 +852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5345AF-81F0-4889-BA58-77C38BD72EEA}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,29 +890,29 @@
       <c r="F1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="20">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="20" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -918,12 +924,12 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
@@ -933,22 +939,22 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="24">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -962,12 +968,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="21"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="9" t="s">
         <v>0</v>
       </c>
@@ -979,22 +985,22 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="20">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="20" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1006,12 +1012,12 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="17"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1021,22 +1027,22 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="24">
         <v>2</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="18" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -1050,12 +1056,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="21"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="13" t="s">
         <v>0</v>
       </c>
@@ -1067,22 +1073,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="20">
+        <v>2</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="17">
-        <v>2</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1096,39 +1102,39 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>50</v>
+      <c r="H11" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="24">
+        <v>3</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="E12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="23">
-        <v>3</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="18" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -1142,39 +1148,39 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="21"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="31" t="s">
-        <v>55</v>
+      <c r="H13" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="20">
+        <v>2</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="E14" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="17">
-        <v>2</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="20" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -1186,12 +1192,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="17"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1200,8 +1206,138 @@
       </c>
       <c r="I15" s="15"/>
     </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="E19" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6">
+        <v>3</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6">
+        <v>4</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6">
+        <v>5</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="11">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="45">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
@@ -1214,37 +1350,6 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1255,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100FDCFF-3743-45D7-B490-C4D0C667DF9C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,14 +1373,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
se agregaron respuestas de posiciones
</commit_message>
<xml_diff>
--- a/robotica-fija/serial_settings.xlsx
+++ b/robotica-fija/serial_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ing-Electronica-ITCG\ing-electronica-itcg\robotica-fija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2CBEE6-47AD-40E9-8B79-F9167AC0359C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC141DD-1494-46DD-BD1E-0418A60360C3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="2" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages Arduino - MatLab" sheetId="1" r:id="rId1"/>
@@ -154,12 +154,6 @@
     <t>Selected JOINT doesn't exist</t>
   </si>
   <si>
-    <t>v1,3</t>
-  </si>
-  <si>
-    <t>Shows selected DOF's configuration</t>
-  </si>
-  <si>
     <t>Read a specific DOF setting</t>
   </si>
   <si>
@@ -215,6 +209,12 @@
   </si>
   <si>
     <t>Attach or Detech an specific servo</t>
+  </si>
+  <si>
+    <t>r1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows selected DOF's configuration  v2,4,54     </t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,50 +442,56 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -854,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5345AF-81F0-4889-BA58-77C38BD72EEA}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B9"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +872,7 @@
     <col min="5" max="5" width="43" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" customWidth="1"/>
     <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="8" max="8" width="41" customWidth="1"/>
+    <col min="8" max="8" width="49.88671875" customWidth="1"/>
     <col min="9" max="9" width="30.21875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
@@ -890,29 +896,29 @@
       <c r="F1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="25">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -924,12 +930,12 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
@@ -939,22 +945,22 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="26">
         <v>3</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="32" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -968,12 +974,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="18"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="9" t="s">
         <v>0</v>
       </c>
@@ -985,22 +991,22 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="25">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="20">
-        <v>1</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1012,12 +1018,12 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="20"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1027,23 +1033,23 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="26">
+        <v>2</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="24">
-        <v>2</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>41</v>
+      <c r="F8" s="33" t="s">
+        <v>60</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>15</v>
@@ -1056,12 +1062,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13" t="s">
         <v>0</v>
       </c>
@@ -1073,22 +1079,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="20">
+      <c r="A10" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="25">
         <v>2</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="20" t="s">
+      <c r="D10" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1102,39 +1108,39 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="20"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="26">
+        <v>3</v>
+      </c>
+      <c r="D12" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="E12" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="24">
-        <v>3</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="32" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -1148,39 +1154,39 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="25">
+        <v>2</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="E14" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="20">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -1192,12 +1198,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1207,14 +1213,14 @@
       <c r="I15" s="15"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="31" t="s">
+      <c r="C19" s="19"/>
+      <c r="E19" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="31"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
@@ -1230,11 +1236,11 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6">
@@ -1305,6 +1311,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G1:I1"/>
@@ -1321,35 +1356,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1360,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100FDCFF-3743-45D7-B490-C4D0C667DF9C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="A1:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,14 +1379,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
Primer version de gui con control
</commit_message>
<xml_diff>
--- a/robotica-fija/serial_settings.xlsx
+++ b/robotica-fija/serial_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ing-Electronica-ITCG\ing-electronica-itcg\robotica-fija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC141DD-1494-46DD-BD1E-0418A60360C3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC994D20-59C1-44F7-8CB3-AE7CAFE7403A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="2" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="1" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages Arduino - MatLab" sheetId="1" r:id="rId1"/>
@@ -445,6 +445,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,39 +492,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5345AF-81F0-4889-BA58-77C38BD72EEA}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,29 +896,29 @@
       <c r="F1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="21">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="21" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -930,12 +930,12 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
@@ -945,22 +945,22 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="25">
         <v>3</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="19" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -974,12 +974,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="27"/>
-      <c r="F5" s="32"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="9" t="s">
         <v>0</v>
       </c>
@@ -991,22 +991,22 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="21">
         <v>1</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="21" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1018,12 +1018,12 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="25"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1033,22 +1033,22 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <v>2</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="28" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -1062,12 +1062,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="27"/>
-      <c r="F9" s="34"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="13" t="s">
         <v>0</v>
       </c>
@@ -1079,22 +1079,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="21">
         <v>2</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="21" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1108,12 +1108,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="25"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1125,22 +1125,22 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="25">
         <v>3</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="19" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -1154,12 +1154,12 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="27"/>
-      <c r="F13" s="32"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="9" t="s">
         <v>0</v>
       </c>
@@ -1171,22 +1171,22 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="21">
         <v>2</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="21" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -1198,12 +1198,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="25"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1213,14 +1213,14 @@
       <c r="I15" s="15"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="E19" s="20" t="s">
+      <c r="C19" s="30"/>
+      <c r="E19" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="31"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
@@ -1311,35 +1311,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G1:I1"/>
@@ -1356,6 +1327,35 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1366,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100FDCFF-3743-45D7-B490-C4D0C667DF9C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1379,14 +1379,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
Se termino primer version de xbox_guide
</commit_message>
<xml_diff>
--- a/robotica-fija/serial_settings.xlsx
+++ b/robotica-fija/serial_settings.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ing-Electronica-ITCG\ing-electronica-itcg\robotica-fija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC994D20-59C1-44F7-8CB3-AE7CAFE7403A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB40E2E0-CA8B-42FA-B492-6EE869DA492B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="1" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="2" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages Arduino - MatLab" sheetId="1" r:id="rId1"/>
     <sheet name="Arduino Serial Commands" sheetId="2" r:id="rId2"/>
-    <sheet name="Serial common expressions" sheetId="3" r:id="rId3"/>
+    <sheet name="Xbox controller" sheetId="4" r:id="rId3"/>
+    <sheet name="Serial common expressions" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
   <si>
     <t>Error code</t>
   </si>
@@ -215,6 +216,105 @@
   </si>
   <si>
     <t xml:space="preserve">Shows selected DOF's configuration  v2,4,54     </t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Move the selected DOF to Home position with an specified Delay time</t>
+  </si>
+  <si>
+    <t>h2,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set SHOULDER_2 HOME_DEGREE by 10 milliseconds between degree </t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>LeftStick</t>
+  </si>
+  <si>
+    <t>RightStick</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>DPadUp</t>
+  </si>
+  <si>
+    <t>DPadDown</t>
+  </si>
+  <si>
+    <t>DPadLeft</t>
+  </si>
+  <si>
+    <t>DPadRight</t>
+  </si>
+  <si>
+    <t>LeftBumper</t>
+  </si>
+  <si>
+    <t>RightBumper</t>
+  </si>
+  <si>
+    <t>Set selected DOF to maped position specified by LeftThumbY</t>
+  </si>
+  <si>
+    <t>Set selected DOF to position without map specified by LeftThumbY, the range in +- 20 degrees</t>
+  </si>
+  <si>
+    <t>Save current Settings in EEPROM</t>
+  </si>
+  <si>
+    <t>Read Settings from EEPROM</t>
+  </si>
+  <si>
+    <t>Set current position HOME_DEGREE</t>
+  </si>
+  <si>
+    <t>Go to HOME_DEGREE</t>
+  </si>
+  <si>
+    <t>Test current DOF</t>
+  </si>
+  <si>
+    <t>Close Settings GUIDE</t>
+  </si>
+  <si>
+    <t>Attach current DOF</t>
+  </si>
+  <si>
+    <t>Dettach Current DOF</t>
+  </si>
+  <si>
+    <t>Move to NEXT DOF settings</t>
+  </si>
+  <si>
+    <t>Move to PREVIOUS DOF settings</t>
+  </si>
+  <si>
+    <t>Set current position MIN_SIGNAL</t>
+  </si>
+  <si>
+    <t>Set current position MAX_SIGNAL</t>
   </si>
 </sst>
 </file>
@@ -391,7 +491,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,13 +546,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -464,34 +585,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -518,6 +639,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>229182</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76597</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04EF1F61-0058-4EF6-89EB-249D60B446C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7299960" y="91440"/>
+          <a:ext cx="6721422" cy="4580017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -860,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5345AF-81F0-4889-BA58-77C38BD72EEA}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,29 +1072,29 @@
       <c r="F1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="26">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -930,12 +1106,12 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
@@ -945,22 +1121,22 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="27">
         <v>3</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="32" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -974,12 +1150,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="19"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="9" t="s">
         <v>0</v>
       </c>
@@ -991,22 +1167,22 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="26">
         <v>1</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1018,12 +1194,12 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="21"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1033,22 +1209,22 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="27">
         <v>2</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="34" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -1062,12 +1238,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="29"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="13" t="s">
         <v>0</v>
       </c>
@@ -1079,22 +1255,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="26">
         <v>2</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1108,12 +1284,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1125,22 +1301,22 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="27">
         <v>3</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="32" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -1154,12 +1330,12 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="19"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="9" t="s">
         <v>0</v>
       </c>
@@ -1171,22 +1347,22 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="26">
         <v>2</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -1198,12 +1374,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1212,17 +1388,63 @@
       </c>
       <c r="I15" s="15"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="27">
+        <v>3</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="19">
+        <v>3</v>
+      </c>
+      <c r="I16" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="E19" s="31" t="s">
+      <c r="C19" s="20"/>
+      <c r="E19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="31"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1461,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1281,7 +1503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1295,7 +1517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1532,42 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="51">
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G1:I1"/>
@@ -1327,35 +1584,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1363,6 +1591,146 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D3379D-A9B7-4C66-8299-362CF256B95D}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100FDCFF-3743-45D7-B490-C4D0C667DF9C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1379,14 +1747,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
xbox guide v 0.8.0
</commit_message>
<xml_diff>
--- a/robotica-fija/serial_settings.xlsx
+++ b/robotica-fija/serial_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ing-Electronica-ITCG\ing-electronica-itcg\robotica-fija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB40E2E0-CA8B-42FA-B492-6EE869DA492B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0793944-4EA2-4BE6-9746-8612A369E765}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="2" xr2:uid="{2CE5BBE7-0D6D-41C2-956C-A860C50A4069}"/>
   </bookViews>
@@ -491,7 +491,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,8 +545,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,24 +607,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -645,16 +639,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>282286</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>128664</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>229182</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76597</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>191397</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>206188</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -683,8 +677,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7299960" y="91440"/>
-          <a:ext cx="6721422" cy="4580017"/>
+          <a:off x="5320451" y="128664"/>
+          <a:ext cx="6005111" cy="4039924"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1072,29 +1066,29 @@
       <c r="F1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="30">
         <v>1</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -1106,12 +1100,12 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1121,22 +1115,22 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="31">
         <v>3</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="36" t="s">
         <v>36</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -1150,12 +1144,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="32"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="9" t="s">
         <v>0</v>
       </c>
@@ -1167,22 +1161,22 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="30">
         <v>1</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1194,12 +1188,12 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="26"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1209,22 +1203,22 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="31">
         <v>2</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="38" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -1238,12 +1232,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="35"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13" t="s">
         <v>0</v>
       </c>
@@ -1255,22 +1249,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="30">
         <v>2</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1284,12 +1278,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1301,22 +1295,22 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="31">
         <v>3</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="36" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -1330,12 +1324,12 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="32"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="9" t="s">
         <v>0</v>
       </c>
@@ -1347,22 +1341,22 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="30">
         <v>2</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -1374,12 +1368,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="26"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1389,60 +1383,60 @@
       <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="31">
         <v>3</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="36" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="22">
         <v>3</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="32"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="E19" s="21" t="s">
+      <c r="C19" s="24"/>
+      <c r="E19" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="21"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
@@ -1594,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D3379D-A9B7-4C66-8299-362CF256B95D}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,122 +1599,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
+    <row r="13" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1747,14 +1741,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>